<commit_message>
Finalized base and nested classifiers, did performance evaluation
</commit_message>
<xml_diff>
--- a/res/ind_train_performance.xlsx
+++ b/res/ind_train_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myfiles/Documents/EPFL/M_I/MLE/scRNAseq/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC22D78-CB63-054B-BF26-C4F87E97264C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF90586F-94D3-0543-BF4F-23EF8B44C7D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="24940" windowHeight="14980" xr2:uid="{8BD3ADAB-721C-7C46-AB94-741A9B76B5D5}"/>
+    <workbookView xWindow="3340" yWindow="1340" windowWidth="24940" windowHeight="14980" xr2:uid="{8BD3ADAB-721C-7C46-AB94-741A9B76B5D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -575,30 +575,30 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>0.95138124379893096</v>
+        <v>0.91143656358648895</v>
       </c>
       <c r="D6">
-        <v>0.77715597646721102</v>
+        <v>0.77744296168747296</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>0.91143656358648895</v>
+        <v>0.95138124379893096</v>
       </c>
       <c r="D7">
-        <v>0.77744296168747296</v>
+        <v>0.77715597646721102</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -617,114 +617,114 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9">
-        <v>0.90091867532662395</v>
+        <v>0.87053819024670798</v>
       </c>
       <c r="D9">
-        <v>0.76797244941885401</v>
+        <v>0.773138183383555</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0.87577581103727697</v>
+        <v>0.83710419463227104</v>
       </c>
       <c r="D10">
-        <v>0.75046635098292402</v>
+        <v>0.77213373511264105</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0.87053819024670798</v>
+        <v>0.86516512560551595</v>
       </c>
       <c r="D11">
-        <v>0.773138183383555</v>
+        <v>0.76983785335055199</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>0.86516512560551595</v>
+        <v>0.83534859386854898</v>
       </c>
       <c r="D12">
-        <v>0.76983785335055199</v>
+        <v>0.76969436074042097</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>0.85611527526492603</v>
+        <v>0.78238329484154401</v>
       </c>
       <c r="D13">
-        <v>0.75548859233749399</v>
+        <v>0.76912039029989898</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>0.83710419463227104</v>
+        <v>0.90091867532662395</v>
       </c>
       <c r="D14">
-        <v>0.77213373511264105</v>
+        <v>0.76797244941885401</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0.83578185577668596</v>
+        <v>0.80482020026846901</v>
       </c>
       <c r="D15">
-        <v>0.76065432630219498</v>
+        <v>0.76739847897833202</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>0.83534859386854898</v>
+        <v>0.67953843203628495</v>
       </c>
       <c r="D16">
-        <v>0.76969436074042097</v>
+        <v>0.767254986368202</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -732,13 +732,13 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>0.83520218611127295</v>
+        <v>0.82084476275439999</v>
       </c>
       <c r="D17">
-        <v>0.76352417850480703</v>
+        <v>0.76438513416558995</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -746,27 +746,27 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>0.82084476275439999</v>
+        <v>0.83520218611127295</v>
       </c>
       <c r="D18">
-        <v>0.76438513416558995</v>
+        <v>0.76352417850480703</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>0.80482020026846901</v>
+        <v>0.83578185577668596</v>
       </c>
       <c r="D19">
-        <v>0.76739847897833202</v>
+        <v>0.76065432630219498</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -785,30 +785,30 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>0.78238329484154401</v>
+        <v>0.85611527526492603</v>
       </c>
       <c r="D21">
-        <v>0.76912039029989898</v>
+        <v>0.75548859233749399</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>0.76763296342307297</v>
+        <v>0.87577581103727697</v>
       </c>
       <c r="D22">
-        <v>0.68890802123690598</v>
+        <v>0.75046635098292402</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -827,30 +827,30 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>0.68349431794495497</v>
+        <v>0.76763296342307297</v>
       </c>
       <c r="D24">
-        <v>0.62491031711866796</v>
+        <v>0.68890802123690598</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25">
-        <v>0.67953843203628495</v>
+        <v>0.65055815873068801</v>
       </c>
       <c r="D25">
-        <v>0.767254986368202</v>
+        <v>0.65733964700817904</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -858,27 +858,27 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>0.67654641109230496</v>
+        <v>0.68349431794495497</v>
       </c>
       <c r="D26">
-        <v>0.56263452432199701</v>
+        <v>0.62491031711866796</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>0.66923286003718496</v>
+        <v>0.63452213208380903</v>
       </c>
       <c r="D27">
-        <v>0.55273353422298699</v>
+        <v>0.57640981489453202</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -886,13 +886,13 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>0.65055815873068801</v>
+        <v>0.67654641109230496</v>
       </c>
       <c r="D28">
-        <v>0.65733964700817904</v>
+        <v>0.56263452432199701</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -900,38 +900,38 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C29">
-        <v>0.63452213208380903</v>
+        <v>0.49974153528043402</v>
       </c>
       <c r="D29">
-        <v>0.57640981489453202</v>
+        <v>0.55517290859520696</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30">
-        <v>0.59138416194899002</v>
+        <v>0.39757101526609301</v>
       </c>
       <c r="D30">
-        <v>0.44482709140479199</v>
+        <v>0.55517290859520696</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>0.49974153528043402</v>
+        <v>0.35197971468829897</v>
       </c>
       <c r="D31">
         <v>0.55517290859520696</v>
@@ -939,16 +939,16 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C32">
-        <v>0.39757101526609301</v>
+        <v>0.66923286003718496</v>
       </c>
       <c r="D32">
-        <v>0.55517290859520696</v>
+        <v>0.55273353422298699</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -970,19 +970,19 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C34">
-        <v>0.35197971468829897</v>
+        <v>0.59138416194899002</v>
       </c>
       <c r="D34">
-        <v>0.55517290859520696</v>
+        <v>0.44482709140479199</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D34" xr:uid="{0F33ADDC-C2AD-0841-BE34-DD551E8B834D}">
     <sortState ref="A2:D34">
-      <sortCondition descending="1" ref="C1:C34"/>
+      <sortCondition descending="1" ref="D1:D34"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Before converting into functions
</commit_message>
<xml_diff>
--- a/res/ind_train_performance.xlsx
+++ b/res/ind_train_performance.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myfiles/Documents/EPFL/M_I/MLE/scRNAseq/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F32228-423D-0F4A-A44A-41C30E080652}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FB5A3F-1907-9B42-9307-B3E2E1DD4206}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="940" windowWidth="24940" windowHeight="14980" xr2:uid="{8BD3ADAB-721C-7C46-AB94-741A9B76B5D5}"/>
+    <workbookView xWindow="240" yWindow="1800" windowWidth="24940" windowHeight="14980" xr2:uid="{8BD3ADAB-721C-7C46-AB94-741A9B76B5D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$D$42</definedName>
-    <definedName name="ind_train_performance_summary" localSheetId="0">Tabelle1!$A$2:$D$42</definedName>
+    <definedName name="ind_train_performance_summary_1" localSheetId="0">Tabelle1!$A$2:$D$42</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{E0BD7DA7-6CA0-DE46-A53D-9C43481CC6A5}" name="ind_train_performance_summary" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{57529B30-4574-A04A-B36D-A6EAB297604B}" name="ind_train_performance_summary" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/myfiles/Documents/EPFL/M_I/MLE/scRNAseq/res/ind_train_performance_summary.csv" thousands="'" comma="1">
       <textFields count="4">
         <textField/>
@@ -73,12 +73,6 @@
     <t>gbf_lowpass</t>
   </si>
   <si>
-    <t>gs_highpass</t>
-  </si>
-  <si>
-    <t>gs_lowpass</t>
-  </si>
-  <si>
     <t>nested</t>
   </si>
   <si>
@@ -101,6 +95,12 @@
   </si>
   <si>
     <t>gs-ref_lowpass</t>
+  </si>
+  <si>
+    <t>filter_and_pca_high-pass</t>
+  </si>
+  <si>
+    <t>filter_and_pca_low-pass</t>
   </si>
 </sst>
 </file>
@@ -138,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -170,14 +170,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -196,7 +207,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ind_train_performance_summary" connectionId="1" xr16:uid="{96D6E747-1709-FD45-9CB9-FA73D7E4FA3F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ind_train_performance_summary_1" connectionId="1" xr16:uid="{97C834B3-A682-2745-8886-B33C0EC6FC55}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -499,89 +510,89 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0.99940628152644195</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0.99311235471373205</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>0.99287329392441104</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.95637824652030401</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>0.98885425091087897</v>
+        <v>0.99928121795245906</v>
       </c>
       <c r="D5">
-        <v>0.95551729085951997</v>
+        <v>0.99641268474673494</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -595,44 +606,44 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7">
-        <v>0.92883469930548002</v>
+        <v>0.95138124379893096</v>
       </c>
       <c r="D7">
-        <v>0.793370641411967</v>
+        <v>0.77715597646721102</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>0.91143656358648895</v>
+        <v>0.92883469930548002</v>
       </c>
       <c r="D8">
-        <v>0.77744296168747296</v>
+        <v>0.793370641411967</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>0.95138124379893096</v>
+        <v>0.91143656358648895</v>
       </c>
       <c r="D9">
-        <v>0.77715597646721102</v>
+        <v>0.77744296168747296</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -651,310 +662,310 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>0.85244349210848802</v>
+        <v>0.90091867532662395</v>
       </c>
       <c r="D11">
-        <v>0.77500358731525298</v>
+        <v>0.76797244941885401</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12">
-        <v>0.87053819024670798</v>
+        <v>0.87577581103727697</v>
       </c>
       <c r="D12">
-        <v>0.773138183383555</v>
+        <v>0.75046635098292402</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>0.83710419463227104</v>
+        <v>0.87316802708043195</v>
       </c>
       <c r="D13">
-        <v>0.77213373511264105</v>
+        <v>0.77084230162146605</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14">
-        <v>0.87316802708043195</v>
+        <v>0.87053819024670798</v>
       </c>
       <c r="D14">
-        <v>0.77084230162146605</v>
+        <v>0.773138183383555</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>0.86544193298259897</v>
+      </c>
+      <c r="D15">
+        <v>0.77342516860381605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15">
+      <c r="B16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4">
         <v>0.86516512560551595</v>
       </c>
-      <c r="D15">
+      <c r="D16" s="4">
         <v>0.76983785335055199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>0.83534859386854898</v>
-      </c>
-      <c r="D16">
-        <v>0.76969436074042097</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>0.78238329484154401</v>
+        <v>0.85611527526492603</v>
       </c>
       <c r="D17">
-        <v>0.76912039029989898</v>
+        <v>0.75548859233749399</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>0.90091867532662395</v>
+        <v>0.85244349210848802</v>
       </c>
       <c r="D18">
-        <v>0.76797244941885401</v>
+        <v>0.77500358731525298</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>0.80482020026846901</v>
+        <v>0.84598962806093003</v>
       </c>
       <c r="D19">
-        <v>0.76739847897833202</v>
+        <v>0.76323719328454498</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>0.67953843203628495</v>
+        <v>0.83710419463227104</v>
       </c>
       <c r="D20">
-        <v>0.767254986368202</v>
+        <v>0.77213373511264105</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>0.82084476275439999</v>
+        <v>0.83578185577668596</v>
       </c>
       <c r="D21">
-        <v>0.76438513416558995</v>
+        <v>0.76065432630219498</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>0.83520218611127295</v>
+        <v>0.83534859386854898</v>
       </c>
       <c r="D22">
-        <v>0.76352417850480703</v>
+        <v>0.76969436074042097</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23">
-        <v>0.83578185577668596</v>
+        <v>0.83520218611127295</v>
       </c>
       <c r="D23">
-        <v>0.76065432630219498</v>
+        <v>0.76352417850480703</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>0.79239659326824397</v>
+        <v>0.82927212999941602</v>
       </c>
       <c r="D24">
-        <v>0.75692351843880001</v>
+        <v>0.76840292724924597</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25">
-        <v>0.85611527526492603</v>
+        <v>0.82625605516137302</v>
       </c>
       <c r="D25">
-        <v>0.75548859233749399</v>
+        <v>0.76782895680872398</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26">
-        <v>0.87577581103727697</v>
+        <v>0.82084476275439999</v>
       </c>
       <c r="D26">
-        <v>0.75046635098292402</v>
+        <v>0.76438513416558995</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C27">
-        <v>0.77432903392557795</v>
+        <v>0.80868937543251096</v>
       </c>
       <c r="D27">
-        <v>0.74156980915482795</v>
+        <v>0.76352417850480703</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>0.80387955544068201</v>
+        <v>0.80547178148892296</v>
       </c>
       <c r="D28">
-        <v>0.73080786339503501</v>
+        <v>0.72449418854928904</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>0.80547178148892296</v>
+        <v>0.80482020026846901</v>
       </c>
       <c r="D29">
-        <v>0.72449418854928904</v>
+        <v>0.76739847897833202</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="C30">
-        <v>0.73822776578093796</v>
+        <v>0.80387955544068201</v>
       </c>
       <c r="D30">
-        <v>0.71416272061988795</v>
+        <v>0.73080786339503501</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C31">
-        <v>0.76763296342307297</v>
+        <v>0.79239659326824397</v>
       </c>
       <c r="D31">
-        <v>0.68890802123690598</v>
+        <v>0.75692351843880001</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32">
-        <v>0.65055815873068801</v>
+        <v>0.78424069735448798</v>
       </c>
       <c r="D32">
-        <v>0.65733964700817904</v>
+        <v>0.76237623762376205</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -962,41 +973,41 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33">
-        <v>0.68349431794495497</v>
+        <v>0.78238329484154401</v>
       </c>
       <c r="D33">
-        <v>0.62491031711866796</v>
+        <v>0.76912039029989898</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>0.63452213208380903</v>
+        <v>0.77563236311791794</v>
       </c>
       <c r="D34">
-        <v>0.57640981489453202</v>
+        <v>0.76381116372506797</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>0.67654641109230496</v>
+        <v>0.77432903392557795</v>
       </c>
       <c r="D35">
-        <v>0.56263452432199701</v>
+        <v>0.74156980915482795</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1004,41 +1015,41 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>0.49974153528043402</v>
+        <v>0.76763296342307297</v>
       </c>
       <c r="D36">
-        <v>0.55517290859520696</v>
+        <v>0.68890802123690598</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>0.5</v>
+        <v>0.73822776578093796</v>
       </c>
       <c r="D37">
-        <v>0.55517290859520696</v>
+        <v>0.71416272061988795</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C38">
-        <v>0.35197971468829897</v>
+        <v>0.68726023228474398</v>
       </c>
       <c r="D38">
-        <v>0.55517290859520696</v>
+        <v>0.74745300617018195</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1046,61 +1057,61 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>0.39757101526609301</v>
+        <v>0.67953843203628495</v>
       </c>
       <c r="D39">
-        <v>0.55517290859520696</v>
+        <v>0.767254986368202</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>0.66923286003718496</v>
+        <v>0.63452213208380903</v>
       </c>
       <c r="D40">
-        <v>0.55273353422298699</v>
+        <v>0.57640981489453202</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C41">
-        <v>0.38261416219911698</v>
+        <v>0.5</v>
       </c>
       <c r="D41">
-        <v>0.46922083512699098</v>
+        <v>0.55517290859520696</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="A42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C42">
-        <v>0.59138416194899002</v>
-      </c>
-      <c r="D42">
-        <v>0.44482709140479199</v>
+      <c r="C42" s="4">
+        <v>0.49974153528043402</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.55517290859520696</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D42" xr:uid="{0F33ADDC-C2AD-0841-BE34-DD551E8B834D}">
     <sortState ref="A2:D42">
-      <sortCondition descending="1" ref="D1:D42"/>
+      <sortCondition descending="1" ref="C1:C42"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>